<commit_message>
2023/10/1 WANGKANG 1. 优化目录结构
</commit_message>
<xml_diff>
--- a/flant5-base-hotpot-fewshot.xlsx
+++ b/flant5-base-hotpot-fewshot.xlsx
@@ -604,7 +604,7 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>unanswerable:information sufficiency</t>
+          <t>unanswerable:other</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -612,7 +612,11 @@
           <t>0</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr"/>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>2222222222</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -683,7 +687,7 @@
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>unanswerable:other</t>
+          <t>answerable</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -691,10 +695,8 @@
           <t>0</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>233</t>
-        </is>
+      <c r="T3" t="n">
+        <v>233</v>
       </c>
     </row>
     <row r="4">
@@ -769,10 +771,8 @@
           <t>answerable</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="S4" t="n">
+        <v>1</v>
       </c>
       <c r="T4" t="inlineStr"/>
     </row>
@@ -849,7 +849,7 @@
         </is>
       </c>
       <c r="S5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T5" t="inlineStr"/>
     </row>
@@ -926,7 +926,7 @@
         </is>
       </c>
       <c r="S6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T6" t="inlineStr"/>
     </row>
@@ -999,7 +999,7 @@
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>unanswerable:understandability</t>
+          <t>answerable</t>
         </is>
       </c>
       <c r="S7" t="n">
@@ -1076,13 +1076,15 @@
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>unanswerable:specificity</t>
+          <t>answerable</t>
         </is>
       </c>
       <c r="S8" t="n">
-        <v>0</v>
-      </c>
-      <c r="T8" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="T8" t="n">
+        <v>1111111111111</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1153,7 +1155,7 @@
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>unanswerable:contextual relevance</t>
+          <t>unanswerable:understandability</t>
         </is>
       </c>
       <c r="S9" t="n">
@@ -1307,13 +1309,17 @@
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>unanswerable:factual consistency</t>
+          <t>unanswerable:other</t>
         </is>
       </c>
       <c r="S11" t="n">
         <v>0</v>
       </c>
-      <c r="T11" t="inlineStr"/>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>1232132123.0</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1467,8 +1473,10 @@
       <c r="S13" t="n">
         <v>0</v>
       </c>
-      <c r="T13" t="n">
-        <v>213213233333</v>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>213213233333.0</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -1540,7 +1548,7 @@
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>answerable</t>
+          <t>unanswerable:information sufficiency</t>
         </is>
       </c>
       <c r="S14" t="n">
@@ -1617,7 +1625,7 @@
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>answerable</t>
+          <t>unanswerable:factual consistency</t>
         </is>
       </c>
       <c r="S15" t="n">
@@ -1692,8 +1700,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R16" t="inlineStr"/>
-      <c r="S16" t="inlineStr"/>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>unanswerable:contextual relevance</t>
+        </is>
+      </c>
+      <c r="S16" t="n">
+        <v>0</v>
+      </c>
       <c r="T16" t="inlineStr"/>
     </row>
     <row r="17">
@@ -1763,8 +1777,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R17" t="inlineStr"/>
-      <c r="S17" t="inlineStr"/>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>unanswerable:specificity</t>
+        </is>
+      </c>
+      <c r="S17" t="n">
+        <v>0</v>
+      </c>
       <c r="T17" t="inlineStr"/>
     </row>
     <row r="18">
@@ -1834,8 +1854,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R18" t="inlineStr"/>
-      <c r="S18" t="inlineStr"/>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>unanswerable:understandability</t>
+        </is>
+      </c>
+      <c r="S18" t="n">
+        <v>0</v>
+      </c>
       <c r="T18" t="inlineStr"/>
     </row>
     <row r="19">
@@ -1905,9 +1931,19 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R19" t="inlineStr"/>
-      <c r="S19" t="inlineStr"/>
-      <c r="T19" t="inlineStr"/>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>unanswerable:other</t>
+        </is>
+      </c>
+      <c r="S19" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>啊啊啊啊啊啊啊啊啊啊啊啊</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1976,8 +2012,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R20" t="inlineStr"/>
-      <c r="S20" t="inlineStr"/>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>unanswerable:understandability</t>
+        </is>
+      </c>
+      <c r="S20" t="n">
+        <v>0</v>
+      </c>
       <c r="T20" t="inlineStr"/>
     </row>
     <row r="21">
@@ -2047,8 +2089,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R21" t="inlineStr"/>
-      <c r="S21" t="inlineStr"/>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S21" t="n">
+        <v>1</v>
+      </c>
       <c r="T21" t="inlineStr"/>
     </row>
     <row r="22">
@@ -2118,8 +2166,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R22" t="inlineStr"/>
-      <c r="S22" t="inlineStr"/>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S22" t="n">
+        <v>1</v>
+      </c>
       <c r="T22" t="inlineStr"/>
     </row>
     <row r="23">
@@ -2189,8 +2243,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R23" t="inlineStr"/>
-      <c r="S23" t="inlineStr"/>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S23" t="n">
+        <v>1</v>
+      </c>
       <c r="T23" t="inlineStr"/>
     </row>
     <row r="24">
@@ -2260,8 +2320,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R24" t="inlineStr"/>
-      <c r="S24" t="inlineStr"/>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S24" t="n">
+        <v>1</v>
+      </c>
       <c r="T24" t="inlineStr"/>
     </row>
     <row r="25">
@@ -2331,8 +2397,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R25" t="inlineStr"/>
-      <c r="S25" t="inlineStr"/>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S25" t="n">
+        <v>1</v>
+      </c>
       <c r="T25" t="inlineStr"/>
     </row>
     <row r="26">
@@ -2402,8 +2474,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R26" t="inlineStr"/>
-      <c r="S26" t="inlineStr"/>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S26" t="n">
+        <v>1</v>
+      </c>
       <c r="T26" t="inlineStr"/>
     </row>
     <row r="27">
@@ -2473,8 +2551,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R27" t="inlineStr"/>
-      <c r="S27" t="inlineStr"/>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S27" t="n">
+        <v>1</v>
+      </c>
       <c r="T27" t="inlineStr"/>
     </row>
     <row r="28">
@@ -2544,8 +2628,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R28" t="inlineStr"/>
-      <c r="S28" t="inlineStr"/>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S28" t="n">
+        <v>1</v>
+      </c>
       <c r="T28" t="inlineStr"/>
     </row>
     <row r="29">
@@ -2615,8 +2705,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R29" t="inlineStr"/>
-      <c r="S29" t="inlineStr"/>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S29" t="n">
+        <v>1</v>
+      </c>
       <c r="T29" t="inlineStr"/>
     </row>
     <row r="30">
@@ -2686,8 +2782,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R30" t="inlineStr"/>
-      <c r="S30" t="inlineStr"/>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S30" t="n">
+        <v>1</v>
+      </c>
       <c r="T30" t="inlineStr"/>
     </row>
     <row r="31">
@@ -2757,8 +2859,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R31" t="inlineStr"/>
-      <c r="S31" t="inlineStr"/>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S31" t="n">
+        <v>1</v>
+      </c>
       <c r="T31" t="inlineStr"/>
     </row>
     <row r="32">
@@ -2828,8 +2936,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R32" t="inlineStr"/>
-      <c r="S32" t="inlineStr"/>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S32" t="n">
+        <v>1</v>
+      </c>
       <c r="T32" t="inlineStr"/>
     </row>
     <row r="33">
@@ -2899,8 +3013,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R33" t="inlineStr"/>
-      <c r="S33" t="inlineStr"/>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S33" t="n">
+        <v>1</v>
+      </c>
       <c r="T33" t="inlineStr"/>
     </row>
     <row r="34">
@@ -2970,8 +3090,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R34" t="inlineStr"/>
-      <c r="S34" t="inlineStr"/>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S34" t="n">
+        <v>1</v>
+      </c>
       <c r="T34" t="inlineStr"/>
     </row>
     <row r="35">
@@ -3041,8 +3167,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R35" t="inlineStr"/>
-      <c r="S35" t="inlineStr"/>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S35" t="n">
+        <v>1</v>
+      </c>
       <c r="T35" t="inlineStr"/>
     </row>
     <row r="36">
@@ -3112,8 +3244,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R36" t="inlineStr"/>
-      <c r="S36" t="inlineStr"/>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S36" t="n">
+        <v>1</v>
+      </c>
       <c r="T36" t="inlineStr"/>
     </row>
     <row r="37">
@@ -3183,8 +3321,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R37" t="inlineStr"/>
-      <c r="S37" t="inlineStr"/>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S37" t="n">
+        <v>1</v>
+      </c>
       <c r="T37" t="inlineStr"/>
     </row>
     <row r="38">
@@ -3254,8 +3398,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R38" t="inlineStr"/>
-      <c r="S38" t="inlineStr"/>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S38" t="n">
+        <v>1</v>
+      </c>
       <c r="T38" t="inlineStr"/>
     </row>
     <row r="39">
@@ -3325,8 +3475,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R39" t="inlineStr"/>
-      <c r="S39" t="inlineStr"/>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S39" t="n">
+        <v>1</v>
+      </c>
       <c r="T39" t="inlineStr"/>
     </row>
     <row r="40">
@@ -3396,8 +3552,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R40" t="inlineStr"/>
-      <c r="S40" t="inlineStr"/>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S40" t="n">
+        <v>1</v>
+      </c>
       <c r="T40" t="inlineStr"/>
     </row>
     <row r="41">
@@ -3467,8 +3629,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R41" t="inlineStr"/>
-      <c r="S41" t="inlineStr"/>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S41" t="n">
+        <v>1</v>
+      </c>
       <c r="T41" t="inlineStr"/>
     </row>
     <row r="42">
@@ -3538,8 +3706,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R42" t="inlineStr"/>
-      <c r="S42" t="inlineStr"/>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S42" t="n">
+        <v>1</v>
+      </c>
       <c r="T42" t="inlineStr"/>
     </row>
     <row r="43">
@@ -3609,8 +3783,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R43" t="inlineStr"/>
-      <c r="S43" t="inlineStr"/>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S43" t="n">
+        <v>1</v>
+      </c>
       <c r="T43" t="inlineStr"/>
     </row>
     <row r="44">
@@ -3680,8 +3860,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R44" t="inlineStr"/>
-      <c r="S44" t="inlineStr"/>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S44" t="n">
+        <v>1</v>
+      </c>
       <c r="T44" t="inlineStr"/>
     </row>
     <row r="45">
@@ -3751,8 +3937,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R45" t="inlineStr"/>
-      <c r="S45" t="inlineStr"/>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S45" t="n">
+        <v>1</v>
+      </c>
       <c r="T45" t="inlineStr"/>
     </row>
     <row r="46">
@@ -3822,8 +4014,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R46" t="inlineStr"/>
-      <c r="S46" t="inlineStr"/>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S46" t="n">
+        <v>1</v>
+      </c>
       <c r="T46" t="inlineStr"/>
     </row>
     <row r="47">
@@ -3893,8 +4091,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R47" t="inlineStr"/>
-      <c r="S47" t="inlineStr"/>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S47" t="n">
+        <v>1</v>
+      </c>
       <c r="T47" t="inlineStr"/>
     </row>
     <row r="48">
@@ -3964,8 +4168,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R48" t="inlineStr"/>
-      <c r="S48" t="inlineStr"/>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S48" t="n">
+        <v>1</v>
+      </c>
       <c r="T48" t="inlineStr"/>
     </row>
     <row r="49">
@@ -4035,8 +4245,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R49" t="inlineStr"/>
-      <c r="S49" t="inlineStr"/>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S49" t="n">
+        <v>1</v>
+      </c>
       <c r="T49" t="inlineStr"/>
     </row>
     <row r="50">
@@ -4106,8 +4322,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R50" t="inlineStr"/>
-      <c r="S50" t="inlineStr"/>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S50" t="n">
+        <v>1</v>
+      </c>
       <c r="T50" t="inlineStr"/>
     </row>
     <row r="51">
@@ -4177,8 +4399,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R51" t="inlineStr"/>
-      <c r="S51" t="inlineStr"/>
+      <c r="R51" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S51" t="n">
+        <v>1</v>
+      </c>
       <c r="T51" t="inlineStr"/>
     </row>
     <row r="52">
@@ -4248,8 +4476,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R52" t="inlineStr"/>
-      <c r="S52" t="inlineStr"/>
+      <c r="R52" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S52" t="n">
+        <v>1</v>
+      </c>
       <c r="T52" t="inlineStr"/>
     </row>
     <row r="53">
@@ -4319,8 +4553,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R53" t="inlineStr"/>
-      <c r="S53" t="inlineStr"/>
+      <c r="R53" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S53" t="n">
+        <v>1</v>
+      </c>
       <c r="T53" t="inlineStr"/>
     </row>
     <row r="54">
@@ -4390,8 +4630,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R54" t="inlineStr"/>
-      <c r="S54" t="inlineStr"/>
+      <c r="R54" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S54" t="n">
+        <v>1</v>
+      </c>
       <c r="T54" t="inlineStr"/>
     </row>
     <row r="55">
@@ -4461,8 +4707,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R55" t="inlineStr"/>
-      <c r="S55" t="inlineStr"/>
+      <c r="R55" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S55" t="n">
+        <v>1</v>
+      </c>
       <c r="T55" t="inlineStr"/>
     </row>
     <row r="56">
@@ -4532,8 +4784,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R56" t="inlineStr"/>
-      <c r="S56" t="inlineStr"/>
+      <c r="R56" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S56" t="n">
+        <v>1</v>
+      </c>
       <c r="T56" t="inlineStr"/>
     </row>
     <row r="57">
@@ -4603,8 +4861,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R57" t="inlineStr"/>
-      <c r="S57" t="inlineStr"/>
+      <c r="R57" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S57" t="n">
+        <v>1</v>
+      </c>
       <c r="T57" t="inlineStr"/>
     </row>
     <row r="58">
@@ -4674,8 +4938,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R58" t="inlineStr"/>
-      <c r="S58" t="inlineStr"/>
+      <c r="R58" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S58" t="n">
+        <v>1</v>
+      </c>
       <c r="T58" t="inlineStr"/>
     </row>
     <row r="59">
@@ -4745,8 +5015,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R59" t="inlineStr"/>
-      <c r="S59" t="inlineStr"/>
+      <c r="R59" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S59" t="n">
+        <v>1</v>
+      </c>
       <c r="T59" t="inlineStr"/>
     </row>
     <row r="60">
@@ -4816,8 +5092,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R60" t="inlineStr"/>
-      <c r="S60" t="inlineStr"/>
+      <c r="R60" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S60" t="n">
+        <v>1</v>
+      </c>
       <c r="T60" t="inlineStr"/>
     </row>
     <row r="61">
@@ -4887,8 +5169,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R61" t="inlineStr"/>
-      <c r="S61" t="inlineStr"/>
+      <c r="R61" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S61" t="n">
+        <v>1</v>
+      </c>
       <c r="T61" t="inlineStr"/>
     </row>
     <row r="62">
@@ -4958,8 +5246,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R62" t="inlineStr"/>
-      <c r="S62" t="inlineStr"/>
+      <c r="R62" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S62" t="n">
+        <v>1</v>
+      </c>
       <c r="T62" t="inlineStr"/>
     </row>
     <row r="63">
@@ -5029,8 +5323,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R63" t="inlineStr"/>
-      <c r="S63" t="inlineStr"/>
+      <c r="R63" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S63" t="n">
+        <v>1</v>
+      </c>
       <c r="T63" t="inlineStr"/>
     </row>
     <row r="64">
@@ -5100,8 +5400,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R64" t="inlineStr"/>
-      <c r="S64" t="inlineStr"/>
+      <c r="R64" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S64" t="n">
+        <v>1</v>
+      </c>
       <c r="T64" t="inlineStr"/>
     </row>
     <row r="65">
@@ -5171,8 +5477,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R65" t="inlineStr"/>
-      <c r="S65" t="inlineStr"/>
+      <c r="R65" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S65" t="n">
+        <v>1</v>
+      </c>
       <c r="T65" t="inlineStr"/>
     </row>
     <row r="66">
@@ -5242,8 +5554,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R66" t="inlineStr"/>
-      <c r="S66" t="inlineStr"/>
+      <c r="R66" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S66" t="n">
+        <v>1</v>
+      </c>
       <c r="T66" t="inlineStr"/>
     </row>
     <row r="67">
@@ -5313,8 +5631,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R67" t="inlineStr"/>
-      <c r="S67" t="inlineStr"/>
+      <c r="R67" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S67" t="n">
+        <v>1</v>
+      </c>
       <c r="T67" t="inlineStr"/>
     </row>
     <row r="68">
@@ -5384,8 +5708,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R68" t="inlineStr"/>
-      <c r="S68" t="inlineStr"/>
+      <c r="R68" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S68" t="n">
+        <v>1</v>
+      </c>
       <c r="T68" t="inlineStr"/>
     </row>
     <row r="69">
@@ -5455,8 +5785,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R69" t="inlineStr"/>
-      <c r="S69" t="inlineStr"/>
+      <c r="R69" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S69" t="n">
+        <v>1</v>
+      </c>
       <c r="T69" t="inlineStr"/>
     </row>
     <row r="70">
@@ -5526,8 +5862,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R70" t="inlineStr"/>
-      <c r="S70" t="inlineStr"/>
+      <c r="R70" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S70" t="n">
+        <v>1</v>
+      </c>
       <c r="T70" t="inlineStr"/>
     </row>
     <row r="71">
@@ -5597,8 +5939,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R71" t="inlineStr"/>
-      <c r="S71" t="inlineStr"/>
+      <c r="R71" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S71" t="n">
+        <v>1</v>
+      </c>
       <c r="T71" t="inlineStr"/>
     </row>
     <row r="72">
@@ -5668,8 +6016,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R72" t="inlineStr"/>
-      <c r="S72" t="inlineStr"/>
+      <c r="R72" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S72" t="n">
+        <v>1</v>
+      </c>
       <c r="T72" t="inlineStr"/>
     </row>
     <row r="73">
@@ -5739,8 +6093,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R73" t="inlineStr"/>
-      <c r="S73" t="inlineStr"/>
+      <c r="R73" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S73" t="n">
+        <v>1</v>
+      </c>
       <c r="T73" t="inlineStr"/>
     </row>
     <row r="74">
@@ -5810,8 +6170,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R74" t="inlineStr"/>
-      <c r="S74" t="inlineStr"/>
+      <c r="R74" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S74" t="n">
+        <v>1</v>
+      </c>
       <c r="T74" t="inlineStr"/>
     </row>
     <row r="75">
@@ -5881,8 +6247,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R75" t="inlineStr"/>
-      <c r="S75" t="inlineStr"/>
+      <c r="R75" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S75" t="n">
+        <v>1</v>
+      </c>
       <c r="T75" t="inlineStr"/>
     </row>
     <row r="76">
@@ -5952,8 +6324,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R76" t="inlineStr"/>
-      <c r="S76" t="inlineStr"/>
+      <c r="R76" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S76" t="n">
+        <v>1</v>
+      </c>
       <c r="T76" t="inlineStr"/>
     </row>
     <row r="77">
@@ -6023,8 +6401,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R77" t="inlineStr"/>
-      <c r="S77" t="inlineStr"/>
+      <c r="R77" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S77" t="n">
+        <v>1</v>
+      </c>
       <c r="T77" t="inlineStr"/>
     </row>
     <row r="78">
@@ -6094,8 +6478,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R78" t="inlineStr"/>
-      <c r="S78" t="inlineStr"/>
+      <c r="R78" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S78" t="n">
+        <v>1</v>
+      </c>
       <c r="T78" t="inlineStr"/>
     </row>
     <row r="79">
@@ -6165,8 +6555,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R79" t="inlineStr"/>
-      <c r="S79" t="inlineStr"/>
+      <c r="R79" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S79" t="n">
+        <v>1</v>
+      </c>
       <c r="T79" t="inlineStr"/>
     </row>
     <row r="80">
@@ -6236,8 +6632,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R80" t="inlineStr"/>
-      <c r="S80" t="inlineStr"/>
+      <c r="R80" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S80" t="n">
+        <v>1</v>
+      </c>
       <c r="T80" t="inlineStr"/>
     </row>
     <row r="81">
@@ -6307,8 +6709,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R81" t="inlineStr"/>
-      <c r="S81" t="inlineStr"/>
+      <c r="R81" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S81" t="n">
+        <v>1</v>
+      </c>
       <c r="T81" t="inlineStr"/>
     </row>
     <row r="82">
@@ -6378,8 +6786,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R82" t="inlineStr"/>
-      <c r="S82" t="inlineStr"/>
+      <c r="R82" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S82" t="n">
+        <v>1</v>
+      </c>
       <c r="T82" t="inlineStr"/>
     </row>
     <row r="83">
@@ -6449,8 +6863,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R83" t="inlineStr"/>
-      <c r="S83" t="inlineStr"/>
+      <c r="R83" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S83" t="n">
+        <v>1</v>
+      </c>
       <c r="T83" t="inlineStr"/>
     </row>
     <row r="84">
@@ -6520,8 +6940,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R84" t="inlineStr"/>
-      <c r="S84" t="inlineStr"/>
+      <c r="R84" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S84" t="n">
+        <v>1</v>
+      </c>
       <c r="T84" t="inlineStr"/>
     </row>
     <row r="85">
@@ -6591,8 +7017,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R85" t="inlineStr"/>
-      <c r="S85" t="inlineStr"/>
+      <c r="R85" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S85" t="n">
+        <v>1</v>
+      </c>
       <c r="T85" t="inlineStr"/>
     </row>
     <row r="86">
@@ -6662,8 +7094,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R86" t="inlineStr"/>
-      <c r="S86" t="inlineStr"/>
+      <c r="R86" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S86" t="n">
+        <v>1</v>
+      </c>
       <c r="T86" t="inlineStr"/>
     </row>
     <row r="87">
@@ -6733,8 +7171,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R87" t="inlineStr"/>
-      <c r="S87" t="inlineStr"/>
+      <c r="R87" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S87" t="n">
+        <v>1</v>
+      </c>
       <c r="T87" t="inlineStr"/>
     </row>
     <row r="88">
@@ -6804,8 +7248,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R88" t="inlineStr"/>
-      <c r="S88" t="inlineStr"/>
+      <c r="R88" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S88" t="n">
+        <v>1</v>
+      </c>
       <c r="T88" t="inlineStr"/>
     </row>
     <row r="89">
@@ -6875,8 +7325,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R89" t="inlineStr"/>
-      <c r="S89" t="inlineStr"/>
+      <c r="R89" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S89" t="n">
+        <v>1</v>
+      </c>
       <c r="T89" t="inlineStr"/>
     </row>
     <row r="90">
@@ -6946,8 +7402,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R90" t="inlineStr"/>
-      <c r="S90" t="inlineStr"/>
+      <c r="R90" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S90" t="n">
+        <v>1</v>
+      </c>
       <c r="T90" t="inlineStr"/>
     </row>
     <row r="91">
@@ -7017,8 +7479,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R91" t="inlineStr"/>
-      <c r="S91" t="inlineStr"/>
+      <c r="R91" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S91" t="n">
+        <v>1</v>
+      </c>
       <c r="T91" t="inlineStr"/>
     </row>
     <row r="92">
@@ -7088,8 +7556,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R92" t="inlineStr"/>
-      <c r="S92" t="inlineStr"/>
+      <c r="R92" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S92" t="n">
+        <v>1</v>
+      </c>
       <c r="T92" t="inlineStr"/>
     </row>
     <row r="93">
@@ -7159,8 +7633,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R93" t="inlineStr"/>
-      <c r="S93" t="inlineStr"/>
+      <c r="R93" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S93" t="n">
+        <v>1</v>
+      </c>
       <c r="T93" t="inlineStr"/>
     </row>
     <row r="94">
@@ -7230,8 +7710,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R94" t="inlineStr"/>
-      <c r="S94" t="inlineStr"/>
+      <c r="R94" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S94" t="n">
+        <v>1</v>
+      </c>
       <c r="T94" t="inlineStr"/>
     </row>
     <row r="95">
@@ -7301,8 +7787,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R95" t="inlineStr"/>
-      <c r="S95" t="inlineStr"/>
+      <c r="R95" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S95" t="n">
+        <v>1</v>
+      </c>
       <c r="T95" t="inlineStr"/>
     </row>
     <row r="96">
@@ -7372,8 +7864,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R96" t="inlineStr"/>
-      <c r="S96" t="inlineStr"/>
+      <c r="R96" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S96" t="n">
+        <v>1</v>
+      </c>
       <c r="T96" t="inlineStr"/>
     </row>
     <row r="97">
@@ -7443,8 +7941,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R97" t="inlineStr"/>
-      <c r="S97" t="inlineStr"/>
+      <c r="R97" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S97" t="n">
+        <v>1</v>
+      </c>
       <c r="T97" t="inlineStr"/>
     </row>
     <row r="98">
@@ -7514,8 +8018,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R98" t="inlineStr"/>
-      <c r="S98" t="inlineStr"/>
+      <c r="R98" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S98" t="n">
+        <v>1</v>
+      </c>
       <c r="T98" t="inlineStr"/>
     </row>
     <row r="99">
@@ -7585,8 +8095,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R99" t="inlineStr"/>
-      <c r="S99" t="inlineStr"/>
+      <c r="R99" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S99" t="n">
+        <v>1</v>
+      </c>
       <c r="T99" t="inlineStr"/>
     </row>
     <row r="100">
@@ -7656,8 +8172,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R100" t="inlineStr"/>
-      <c r="S100" t="inlineStr"/>
+      <c r="R100" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S100" t="n">
+        <v>1</v>
+      </c>
       <c r="T100" t="inlineStr"/>
     </row>
     <row r="101">
@@ -7727,8 +8249,14 @@
           <t>HotpotQA-FlanT5base-Fewshot</t>
         </is>
       </c>
-      <c r="R101" t="inlineStr"/>
-      <c r="S101" t="inlineStr"/>
+      <c r="R101" t="inlineStr">
+        <is>
+          <t>answerable</t>
+        </is>
+      </c>
+      <c r="S101" t="n">
+        <v>1</v>
+      </c>
       <c r="T101" t="inlineStr"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2023/10/2 WANGKANG 1. 重构文件结构
</commit_message>
<xml_diff>
--- a/flant5-base-hotpot-fewshot.xlsx
+++ b/flant5-base-hotpot-fewshot.xlsx
@@ -604,7 +604,7 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>unanswerable:other</t>
+          <t>unanswerable:understandability</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -687,7 +687,7 @@
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>answerable</t>
+          <t>unanswerable:other</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -695,8 +695,10 @@
           <t>0</t>
         </is>
       </c>
-      <c r="T3" t="n">
-        <v>233</v>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>啊啊啊啊啊啊啊啊啊啊</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -771,8 +773,10 @@
           <t>answerable</t>
         </is>
       </c>
-      <c r="S4" t="n">
-        <v>1</v>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="T4" t="inlineStr"/>
     </row>

</xml_diff>